<commit_message>
Tested geoparsing on sample, but quite a few errors in location identification.
</commit_message>
<xml_diff>
--- a/data/derived-data/coding/keyword-search-tokens.xlsx
+++ b/data/derived-data/coding/keyword-search-tokens.xlsx
@@ -671,8 +671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B82" sqref="B82"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1718,7 +1718,7 @@
         <v>48</v>
       </c>
       <c r="B75" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C75" t="s">
         <v>87</v>
@@ -1732,7 +1732,7 @@
         <v>48</v>
       </c>
       <c r="B76" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C76" t="s">
         <v>88</v>

</xml_diff>